<commit_message>
Update phoeniX Static Time Analysis excel file
</commit_message>
<xml_diff>
--- a/Documents/phoeniX Static Time Analysis.xlsx
+++ b/Documents/phoeniX Static Time Analysis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Module</t>
   </si>
@@ -67,6 +67,39 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>4ns</t>
+  </si>
+  <si>
+    <t>3 clk cycles</t>
+  </si>
+  <si>
+    <t>CPI (R,I-TYPE)</t>
+  </si>
+  <si>
+    <t>250MHz</t>
+  </si>
+  <si>
+    <t>Core specifications</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>10000 - 40000</t>
+  </si>
+  <si>
+    <t>4KB</t>
+  </si>
+  <si>
+    <t>Memory address space</t>
+  </si>
+  <si>
+    <t>Clock Cycle Time</t>
+  </si>
+  <si>
+    <t>Memory Operation Time</t>
   </si>
 </sst>
 </file>
@@ -96,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -119,11 +152,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -132,6 +191,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -414,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:D16"/>
+  <dimension ref="C3:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,113 +493,163 @@
     <col min="1" max="2" width="8.88671875" customWidth="1"/>
     <col min="3" max="3" width="31.77734375" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="1">
         <v>3844.84</v>
       </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1">
         <v>3099.01</v>
       </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="1">
         <v>747.68899999999996</v>
       </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1">
         <v>1131.73</v>
       </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1">
         <v>1016.44</v>
       </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="1">
         <v>716.43700000000001</v>
       </c>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="1">
         <v>243.11500000000001</v>
       </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="1">
         <v>265.64800000000002</v>
       </c>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="1">
         <v>308.90699999999998</v>
       </c>
-    </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="1">
         <v>569.90300000000002</v>
       </c>
-    </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
         <v>15</v>
       </c>
@@ -539,8 +657,13 @@
         <f>SUM(D4:D15)-D12</f>
         <v>11678.071</v>
       </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:G3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>